<commit_message>
update API new code
</commit_message>
<xml_diff>
--- a/MISA.WEB07.TNANH.MultiLayer.API/Danh sách cán bộ nhân viên.xlsx
+++ b/MISA.WEB07.TNANH.MultiLayer.API/Danh sách cán bộ nhân viên.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <x:si>
     <x:t>DANH SÁCH CÁN BỘ - GIÁO VIÊN</x:t>
   </x:si>
@@ -46,136 +46,106 @@
     <x:t>Đang làm việc</x:t>
   </x:si>
   <x:si>
-    <x:t>NV60276254</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyễn Thái Lệ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>036101320</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tổ Anh - Văn</x:t>
+    <x:t>NV72573840</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Đinh Yên Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>074232234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hóa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>x</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NV92831013</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vũ Kiến Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>044292284</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Tổ Sử Địa </x:t>
+  </x:si>
+  <x:si>
+    <x:t>NV99829582</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lê Ngọc Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>087342212</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tổ Hóa - Sinh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Toán</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NV59507985</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nguyễn Mạnh Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>069309572</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NV66662587</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lê Như Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>031561639</x:t>
   </x:si>
   <x:si>
     <x:t>Văn</x:t>
   </x:si>
   <x:si>
-    <x:t>Phòng hóa sinh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>x</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV57757809</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hoàng Đình Hưng</x:t>
-  </x:si>
-  <x:si>
-    <x:t>000066201</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tổ Hóa - Sinh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hóa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV43079132</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lê Mạnh An</x:t>
-  </x:si>
-  <x:si>
-    <x:t>069992849</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Địa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kho thiết bị chung</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV19273367</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trương Như Nguyệt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>063491850</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Tổ Sử Địa </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sử</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV54790074</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ngô Thái Minh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>064100527</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV27936382</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyễn Ngọc Thái</x:t>
-  </x:si>
-  <x:si>
-    <x:t>092316765</x:t>
+    <x:t>NV18993783</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nguyễn Minh Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>054327222</x:t>
   </x:si>
   <x:si>
     <x:t>Tổ Lý</x:t>
   </x:si>
   <x:si>
-    <x:t>Lý</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV79090193</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hoàng Diễm Nhi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>042687151</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Anh</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Phòng lý</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV34486789</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lê Đăng Trung</x:t>
-  </x:si>
-  <x:si>
-    <x:t>068782823</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV20522621</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Vũ Minh Thuận</x:t>
-  </x:si>
-  <x:si>
-    <x:t>083602931</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NV03728881</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trần Chí Hương</x:t>
-  </x:si>
-  <x:si>
-    <x:t>034373116</x:t>
+    <x:t>NV89320025</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hồ Phương Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>023439844</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NV52112691</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lê Đona Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>034396549</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NV89033488</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vũ Gia Nam</x:t>
+  </x:si>
+  <x:si>
+    <x:t>087350901</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -347,8 +317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:I13" totalsRowShown="0">
-  <x:autoFilter ref="A3:I13"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:I12" totalsRowShown="0">
+  <x:autoFilter ref="A3:I12"/>
   <x:tableColumns count="9">
     <x:tableColumn id="1" name="STT" dataDxfId="0"/>
     <x:tableColumn id="2" name="Số hiệu cán bộ" dataDxfId="1"/>
@@ -652,7 +622,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:I13"/>
+  <x:dimension ref="A1:I12"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -734,20 +704,14 @@
       <x:c r="D4" s="7" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="E4" s="5" t="s">
+      <x:c r="E4" s="5" t="s"/>
+      <x:c r="F4" s="6" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="F4" s="6" t="s">
+      <x:c r="G4" s="6" t="s"/>
+      <x:c r="H4" s="5" t="s"/>
+      <x:c r="I4" s="5" t="s">
         <x:v>14</x:v>
-      </x:c>
-      <x:c r="G4" s="6" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="H4" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I4" s="5" t="s">
-        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:9">
@@ -755,28 +719,22 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B5" s="6" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C5" s="6" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D5" s="7" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C5" s="6" t="s">
+      <x:c r="E5" s="5" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D5" s="7" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E5" s="5" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F5" s="6" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="G5" s="6" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="H5" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
+      <x:c r="F5" s="6" t="s"/>
+      <x:c r="G5" s="6" t="s"/>
+      <x:c r="H5" s="5" t="s"/>
       <x:c r="I5" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:9">
@@ -784,28 +742,24 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B6" s="6" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C6" s="6" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D6" s="7" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E6" s="5" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C6" s="6" t="s">
+      <x:c r="F6" s="6" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="D6" s="7" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="E6" s="5" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="F6" s="6" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="G6" s="6" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="H6" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
+      <x:c r="G6" s="6" t="s"/>
+      <x:c r="H6" s="5" t="s"/>
       <x:c r="I6" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:9">
@@ -813,24 +767,22 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B7" s="6" t="s">
-        <x:v>27</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C7" s="6" t="s">
-        <x:v>28</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D7" s="7" t="s">
-        <x:v>29</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E7" s="5" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F7" s="6" t="s">
-        <x:v>31</x:v>
-      </x:c>
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F7" s="6" t="s"/>
       <x:c r="G7" s="6" t="s"/>
       <x:c r="H7" s="5" t="s"/>
       <x:c r="I7" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:9">
@@ -838,22 +790,24 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B8" s="6" t="s">
-        <x:v>32</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C8" s="6" t="s">
-        <x:v>33</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D8" s="7" t="s">
-        <x:v>34</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="E8" s="5" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="F8" s="6" t="s"/>
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F8" s="6" t="s">
+        <x:v>30</x:v>
+      </x:c>
       <x:c r="G8" s="6" t="s"/>
       <x:c r="H8" s="5" t="s"/>
       <x:c r="I8" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:9">
@@ -861,24 +815,22 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B9" s="6" t="s">
-        <x:v>35</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C9" s="6" t="s">
-        <x:v>36</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="D9" s="7" t="s">
-        <x:v>37</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E9" s="5" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="F9" s="6" t="s">
-        <x:v>39</x:v>
-      </x:c>
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F9" s="6" t="s"/>
       <x:c r="G9" s="6" t="s"/>
       <x:c r="H9" s="5" t="s"/>
       <x:c r="I9" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:9">
@@ -886,28 +838,22 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B10" s="6" t="s">
-        <x:v>40</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C10" s="6" t="s">
-        <x:v>41</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D10" s="7" t="s">
-        <x:v>42</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E10" s="5" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="F10" s="6" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="G10" s="6" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="H10" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F10" s="6" t="s"/>
+      <x:c r="G10" s="6" t="s"/>
+      <x:c r="H10" s="5" t="s"/>
       <x:c r="I10" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:9">
@@ -915,24 +861,24 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B11" s="6" t="s">
-        <x:v>45</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C11" s="6" t="s">
-        <x:v>46</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D11" s="7" t="s">
-        <x:v>47</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E11" s="5" t="s">
-        <x:v>30</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F11" s="6" t="s">
-        <x:v>14</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="G11" s="6" t="s"/>
       <x:c r="H11" s="5" t="s"/>
       <x:c r="I11" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:9">
@@ -940,49 +886,24 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B12" s="6" t="s">
-        <x:v>48</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C12" s="6" t="s">
-        <x:v>49</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D12" s="7" t="s">
-        <x:v>50</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="E12" s="5" t="s">
-        <x:v>20</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F12" s="6" t="s">
-        <x:v>21</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G12" s="6" t="s"/>
       <x:c r="H12" s="5" t="s"/>
       <x:c r="I12" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:9">
-      <x:c r="A13" s="5" t="n">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B13" s="6" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="C13" s="6" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="D13" s="7" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="E13" s="5" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F13" s="6" t="s"/>
-      <x:c r="G13" s="6" t="s"/>
-      <x:c r="H13" s="5" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="I13" s="5" t="s">
-        <x:v>16</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>